<commit_message>
update contracts status to'подписан'
</commit_message>
<xml_diff>
--- a/upload/payment/счет_24546800.xlsx
+++ b/upload/payment/счет_24546800.xlsx
@@ -854,7 +854,7 @@
       <c r="B8" s="10" t="n"/>
       <c r="C8" s="22" t="inlineStr">
         <is>
-          <t>Оплата участия в серии мероприятий для бизнеса "Клуба Первых". По Договору оказания услуг ФЛМ-24546800 от 5.10.21</t>
+          <t>Оплата участия в серии мероприятий для бизнеса "Клуба Первых" Тариф "Продление" по Договору оказания услуг ПМ-24546800 от 26.10.21</t>
         </is>
       </c>
     </row>
@@ -872,7 +872,7 @@
       <c r="B10" s="10" t="n"/>
       <c r="C10" s="8" t="inlineStr">
         <is>
-          <t>123653</t>
+          <t>75000</t>
         </is>
       </c>
     </row>
@@ -975,7 +975,7 @@
       <c r="B21" s="10" t="n"/>
       <c r="C21" s="11" t="inlineStr">
         <is>
-          <t>Оплата участия в серии мероприятий для бизнеса "Клуба Первых". По Договору оказания услуг ФЛМ-24546800 от 5.10.21</t>
+          <t>Оплата участия в серии мероприятий для бизнеса "Клуба Первых" Тариф "Продление" по Договору оказания услуг ПМ-24546800 от 26.10.21</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       <c r="B23" s="5" t="n"/>
       <c r="C23" s="8" t="inlineStr">
         <is>
-          <t>123653</t>
+          <t>75000</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed saving full name
</commit_message>
<xml_diff>
--- a/upload/payment/счет_24546800.xlsx
+++ b/upload/payment/счет_24546800.xlsx
@@ -401,7 +401,7 @@
       <row>17</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1428750" cy="1428750"/>
+    <ext cx="1504950" cy="1504950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -854,7 +854,7 @@
       <c r="B8" s="10" t="n"/>
       <c r="C8" s="22" t="inlineStr">
         <is>
-          <t>Оплата участия в серии мероприятий для бизнеса "Клуба Первых" Тариф "Продление" по Договору оказания услуг ПМ-24546800 от 21.11.21</t>
+          <t>Оплата участия в серии мероприятий для бизнеса "Клуба Первых" Тариф "Продление" по Договору оказания услуг ПМ-24546800 от 19.04.22</t>
         </is>
       </c>
     </row>
@@ -872,7 +872,7 @@
       <c r="B10" s="10" t="n"/>
       <c r="C10" s="8" t="inlineStr">
         <is>
-          <t>78000</t>
+          <t>10000</t>
         </is>
       </c>
     </row>
@@ -975,7 +975,7 @@
       <c r="B21" s="10" t="n"/>
       <c r="C21" s="11" t="inlineStr">
         <is>
-          <t>Оплата участия в серии мероприятий для бизнеса "Клуба Первых" Тариф "Продление" по Договору оказания услуг ПМ-24546800 от 21.11.21</t>
+          <t>Оплата участия в серии мероприятий для бизнеса "Клуба Первых" Тариф "Продление" по Договору оказания услуг ПМ-24546800 от 19.04.22</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       <c r="B23" s="5" t="n"/>
       <c r="C23" s="8" t="inlineStr">
         <is>
-          <t>78000</t>
+          <t>10000</t>
         </is>
       </c>
     </row>

</xml_diff>